<commit_message>
Dynamic relaxation basics added.
</commit_message>
<xml_diff>
--- a/Documentation/Interop Links.xlsx
+++ b/Documentation/Interop Links.xlsx
@@ -468,24 +468,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,9 +476,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -525,12 +504,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,210 +832,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="22" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="30"/>
+      <c r="F3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="5" t="s">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="F4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="H4" s="24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="6">
+      <c r="C5" s="26"/>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="17">
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+      <c r="H5" s="23">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-      <c r="E5" s="24">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="30">
-        <v>1</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9">
-        <v>1</v>
-      </c>
-      <c r="E6" s="25">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9">
-        <v>1</v>
-      </c>
-      <c r="G6" s="28">
-        <v>1</v>
+      <c r="C6" s="15"/>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="18">
+        <v>2</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="21">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="C7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="25">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9">
-        <v>1</v>
-      </c>
-      <c r="G7" s="28"/>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="18">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="21" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="34"/>
+      <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="28"/>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="21">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="25">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="28">
-        <v>1</v>
+      <c r="C9" s="15"/>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="18">
+        <v>2</v>
+      </c>
+      <c r="G9" s="9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="21">
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="19">
-        <v>1</v>
-      </c>
-      <c r="D10" s="20">
-        <v>1</v>
-      </c>
-      <c r="E10" s="26">
-        <v>1</v>
-      </c>
-      <c r="F10" s="20">
-        <v>1</v>
-      </c>
-      <c r="G10" s="28"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="13">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14">
+        <v>2</v>
+      </c>
+      <c r="F10" s="19">
+        <v>2</v>
+      </c>
+      <c r="G10" s="14">
+        <v>2</v>
+      </c>
+      <c r="H10" s="21">
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="10">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="29"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="10">
+        <v>2</v>
+      </c>
+      <c r="E11" s="11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>2</v>
+      </c>
+      <c r="H11" s="22">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:G11">
-    <cfRule type="iconSet" priority="1">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{6D19CFAF-C759-49C8-9C08-DF6467F79E68}">
+            <x14:iconSet iconSet="3Stars" showValue="0">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D5:H11</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Minor curve and interval tweaks
</commit_message>
<xml_diff>
--- a/Documentation/Interop Links.xlsx
+++ b/Documentation/Interop Links.xlsx
@@ -84,12 +84,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="26">
@@ -442,14 +454,6 @@
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -468,17 +472,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,9 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,37 +496,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,7 +847,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,187 +865,187 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="35" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="20" t="s">
+      <c r="G3" s="20"/>
+      <c r="H3" s="21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="27" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="6">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7">
-        <v>2</v>
-      </c>
-      <c r="F5" s="17">
-        <v>2</v>
-      </c>
-      <c r="G5" s="7">
-        <v>2</v>
-      </c>
-      <c r="H5" s="23">
+      <c r="C5" s="29"/>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="8">
-        <v>2</v>
-      </c>
-      <c r="E6" s="9">
-        <v>2</v>
-      </c>
-      <c r="F6" s="18">
-        <v>2</v>
-      </c>
-      <c r="G6" s="9">
-        <v>2</v>
-      </c>
-      <c r="H6" s="21">
+      <c r="C6" s="31"/>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="11">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>0</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F7" s="18">
-        <v>2</v>
-      </c>
-      <c r="G7" s="9">
-        <v>2</v>
-      </c>
-      <c r="H7" s="21">
+      <c r="F7" s="11">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
-      <c r="C8" s="15" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="9">
-        <v>2</v>
-      </c>
-      <c r="F8" s="18">
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11">
         <v>0</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="5">
         <v>0</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="8">
-        <v>2</v>
-      </c>
-      <c r="E9" s="9">
-        <v>2</v>
-      </c>
-      <c r="F9" s="18">
-        <v>2</v>
-      </c>
-      <c r="G9" s="9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="21">
+      <c r="C9" s="31"/>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11">
+        <v>2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2</v>
+      </c>
+      <c r="H9" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="13">
-        <v>2</v>
-      </c>
-      <c r="E10" s="14">
-        <v>2</v>
-      </c>
-      <c r="F10" s="19">
-        <v>2</v>
-      </c>
-      <c r="G10" s="14">
-        <v>2</v>
-      </c>
-      <c r="H10" s="21">
+      <c r="C10" s="34"/>
+      <c r="D10" s="8">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2</v>
+      </c>
+      <c r="F10" s="12">
+        <v>2</v>
+      </c>
+      <c r="G10" s="9">
+        <v>2</v>
+      </c>
+      <c r="H10" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="10">
-        <v>2</v>
-      </c>
-      <c r="E11" s="11">
-        <v>2</v>
-      </c>
-      <c r="F11" s="10">
+      <c r="C11" s="36"/>
+      <c r="D11" s="6">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6">
         <v>0</v>
       </c>
-      <c r="G11" s="11">
-        <v>2</v>
-      </c>
-      <c r="H11" s="22">
+      <c r="G11" s="7">
+        <v>2</v>
+      </c>
+      <c r="H11" s="14">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfixing, curve self-intersection tests & wind calcs started
</commit_message>
<xml_diff>
--- a/Documentation/Interop Links.xlsx
+++ b/Documentation/Interop Links.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="354E431D6995263F49A600CF6100C1A7050825AB" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{38D8E2BC-59F6-462A-B398-E2018FAB86DB}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Current Interoperability Status</t>
   </si>
@@ -83,6 +82,9 @@
   </si>
   <si>
     <t>Thermal</t>
+  </si>
+  <si>
+    <t>Levels</t>
   </si>
 </sst>
 </file>
@@ -126,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -480,6 +482,19 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -551,10 +566,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -580,16 +605,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -930,46 +949,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="35" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="17" t="s">
         <v>3</v>
       </c>
@@ -986,11 +1005,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="37" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="2">
         <v>2</v>
       </c>
@@ -1007,11 +1026,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="27" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="4">
         <v>2</v>
       </c>
@@ -1028,8 +1047,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="34" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="21" t="s">
@@ -1051,8 +1070,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="34"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="36"/>
       <c r="C8" s="21" t="s">
         <v>10</v>
       </c>
@@ -1072,11 +1091,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="27" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="4">
         <v>2</v>
       </c>
@@ -1093,11 +1112,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="8">
         <v>2</v>
       </c>
@@ -1114,11 +1133,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="8">
         <v>2</v>
       </c>
@@ -1131,11 +1150,11 @@
       <c r="G11" s="9">
         <v>2</v>
       </c>
-      <c r="H11" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
         <v>16</v>
       </c>
@@ -1154,11 +1173,11 @@
       <c r="G12" s="9">
         <v>2</v>
       </c>
-      <c r="H12" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="C13" s="23" t="s">
         <v>18</v>
@@ -1175,11 +1194,11 @@
       <c r="G13" s="9">
         <v>2</v>
       </c>
-      <c r="H13" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="22"/>
       <c r="C14" s="23" t="s">
         <v>19</v>
@@ -1196,11 +1215,11 @@
       <c r="G14" s="9">
         <v>2</v>
       </c>
-      <c r="H14" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
       <c r="C15" s="23" t="s">
         <v>20</v>
@@ -1217,11 +1236,11 @@
       <c r="G15" s="9">
         <v>2</v>
       </c>
-      <c r="H15" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="22"/>
       <c r="C16" s="23" t="s">
         <v>21</v>
@@ -1238,42 +1257,65 @@
       <c r="G16" s="9">
         <v>1</v>
       </c>
-      <c r="H16" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="24" t="s">
+      <c r="H16" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>2</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="7">
-        <v>2</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0</v>
-      </c>
-      <c r="G17" s="7">
-        <v>2</v>
-      </c>
-      <c r="H17" s="14">
-        <v>0</v>
+      <c r="C18" s="38"/>
+      <c r="D18" s="6">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2</v>
+      </c>
+      <c r="H18" s="14">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1294,7 +1336,7 @@
               </x14:cfvo>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>D5:H17</xm:sqref>
+          <xm:sqref>D5:H18</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1308,7 +1350,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1320,7 +1362,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>